<commit_message>
new wc in part b
</commit_message>
<xml_diff>
--- a/part_A.xlsx
+++ b/part_A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhild\Desktop\EPFL_progs\IntroFin\IF-case1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C68AC9-C0DF-47EB-8EDD-51E7D0BB5CE9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{669958EF-7AF0-4E1E-A5E1-E1302CFECEC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{83F0B71E-83C5-FB4C-BC89-723A38B8AFA2}"/>
   </bookViews>
@@ -631,7 +631,7 @@
   <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -1177,55 +1177,55 @@
         <v>1</v>
       </c>
       <c r="C18" s="16">
-        <f>C17/B17</f>
+        <f t="shared" ref="C18:O18" si="3">C17/B17</f>
         <v>1.090023752969121</v>
       </c>
       <c r="D18" s="16">
-        <f>D17/C17</f>
+        <f t="shared" si="3"/>
         <v>1.0899760296360863</v>
       </c>
       <c r="E18" s="16">
-        <f>E17/D17</f>
+        <f t="shared" si="3"/>
         <v>1.089865850976629</v>
       </c>
       <c r="F18" s="16">
-        <f>F17/E17</f>
+        <f t="shared" si="3"/>
         <v>1.0900502623179367</v>
       </c>
       <c r="G18" s="16">
-        <f>G17/F17</f>
+        <f t="shared" si="3"/>
         <v>1.0900661360079431</v>
       </c>
       <c r="H18" s="16">
-        <f>H17/G17</f>
+        <f t="shared" si="3"/>
         <v>1.089988421458896</v>
       </c>
       <c r="I18" s="16">
-        <f>I17/H17</f>
+        <f t="shared" si="3"/>
         <v>1.0900515551526826</v>
       </c>
       <c r="J18" s="16">
-        <f>J17/I17</f>
+        <f t="shared" si="3"/>
         <v>1.0899794703879837</v>
       </c>
       <c r="K18" s="16">
-        <f>K17/J17</f>
+        <f t="shared" si="3"/>
         <v>1.0899543433428303</v>
       </c>
       <c r="L18" s="16">
-        <f>L17/K17</f>
+        <f t="shared" si="3"/>
         <v>1.0900331390198288</v>
       </c>
       <c r="M18" s="16">
-        <f>M17/L17</f>
+        <f t="shared" si="3"/>
         <v>1.0900115386544924</v>
       </c>
       <c r="N18" s="16">
-        <f>N17/M17</f>
+        <f t="shared" si="3"/>
         <v>1.0900069958393166</v>
       </c>
       <c r="O18" s="17">
-        <f>O17/N17</f>
+        <f t="shared" si="3"/>
         <v>1.0400206056716268</v>
       </c>
     </row>
@@ -1254,56 +1254,56 @@
         <v>-16.329999999999998</v>
       </c>
       <c r="C20" s="16">
-        <f>$B$20*C18</f>
+        <f>B20*C18</f>
         <v>-17.800087885985743</v>
       </c>
       <c r="D20" s="16">
-        <f>$B$20*D18</f>
-        <v>-17.799308563957286</v>
+        <f t="shared" ref="D20:O20" si="4">C20*D18</f>
+        <v>-19.401669121140138</v>
       </c>
       <c r="E20" s="16">
-        <f>$B$20*E18</f>
-        <v>-17.797509346448351</v>
+        <f t="shared" si="4"/>
+        <v>-21.145216627078383</v>
       </c>
       <c r="F20" s="16">
-        <f>$B$20*F18</f>
-        <v>-17.800520783651905</v>
+        <f t="shared" si="4"/>
+        <v>-23.049348931116388</v>
       </c>
       <c r="G20" s="16">
-        <f>$B$20*G18</f>
-        <v>-17.800780001009709</v>
+        <f t="shared" si="4"/>
+        <v>-25.125314726840855</v>
       </c>
       <c r="H20" s="16">
-        <f>$B$20*H18</f>
-        <v>-17.799510922423771</v>
+        <f t="shared" si="4"/>
+        <v>-27.386302137767217</v>
       </c>
       <c r="I20" s="16">
-        <f>$B$20*I18</f>
-        <v>-17.800541895643306</v>
+        <f t="shared" si="4"/>
+        <v>-29.852481235154389</v>
       </c>
       <c r="J20" s="16">
-        <f>$B$20*J18</f>
-        <v>-17.799364751435771</v>
+        <f t="shared" si="4"/>
+        <v>-32.538591686460805</v>
       </c>
       <c r="K20" s="16">
-        <f>$B$20*K18</f>
-        <v>-17.798954426788416</v>
+        <f t="shared" si="4"/>
+        <v>-35.46557933491686</v>
       </c>
       <c r="L20" s="16">
-        <f>$B$20*L18</f>
-        <v>-17.800241160193803</v>
+        <f t="shared" si="4"/>
+        <v>-38.658656769596199</v>
       </c>
       <c r="M20" s="16">
-        <f>$B$20*M18</f>
-        <v>-17.799888426227859</v>
+        <f t="shared" si="4"/>
+        <v>-42.138381947743461</v>
       </c>
       <c r="N20" s="16">
-        <f>$B$20*N18</f>
-        <v>-17.799814242056037</v>
-      </c>
-      <c r="O20" s="17">
-        <f>$B$20*O18</f>
-        <v>-16.983536490617663</v>
+        <f t="shared" si="4"/>
+        <v>-45.931131116389544</v>
+      </c>
+      <c r="O20" s="16">
+        <f t="shared" si="4"/>
+        <v>-47.769322802850354</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.6">
@@ -1316,52 +1316,52 @@
         <v>-1.4700878859857447</v>
       </c>
       <c r="D21" s="19">
-        <f t="shared" ref="D21:O21" si="3">D20-C20</f>
-        <v>7.793220284568747E-4</v>
+        <f t="shared" ref="D21:O21" si="5">D20-C20</f>
+        <v>-1.601581235154395</v>
       </c>
       <c r="E21" s="19">
-        <f t="shared" si="3"/>
-        <v>1.7992175089354134E-3</v>
+        <f t="shared" si="5"/>
+        <v>-1.7435475059382455</v>
       </c>
       <c r="F21" s="19">
-        <f t="shared" si="3"/>
-        <v>-3.0114372035541237E-3</v>
+        <f t="shared" si="5"/>
+        <v>-1.9041323040380043</v>
       </c>
       <c r="G21" s="19">
-        <f t="shared" si="3"/>
-        <v>-2.59217357804431E-4</v>
+        <f t="shared" si="5"/>
+        <v>-2.0759657957244677</v>
       </c>
       <c r="H21" s="19">
-        <f t="shared" si="3"/>
-        <v>1.269078585938388E-3</v>
+        <f t="shared" si="5"/>
+        <v>-2.2609874109263615</v>
       </c>
       <c r="I21" s="19">
-        <f t="shared" si="3"/>
-        <v>-1.0309732195352694E-3</v>
+        <f t="shared" si="5"/>
+        <v>-2.4661790973871724</v>
       </c>
       <c r="J21" s="19">
-        <f t="shared" si="3"/>
-        <v>1.177144207535008E-3</v>
+        <f t="shared" si="5"/>
+        <v>-2.6861104513064156</v>
       </c>
       <c r="K21" s="19">
-        <f t="shared" si="3"/>
-        <v>4.1032464735479834E-4</v>
+        <f t="shared" si="5"/>
+        <v>-2.9269876484560555</v>
       </c>
       <c r="L21" s="19">
-        <f t="shared" si="3"/>
-        <v>-1.286733405386542E-3</v>
+        <f t="shared" si="5"/>
+        <v>-3.1930774346793385</v>
       </c>
       <c r="M21" s="19">
-        <f t="shared" si="3"/>
-        <v>3.5273396594348583E-4</v>
+        <f t="shared" si="5"/>
+        <v>-3.4797251781472625</v>
       </c>
       <c r="N21" s="19">
-        <f t="shared" si="3"/>
-        <v>7.4184171822366807E-5</v>
+        <f t="shared" si="5"/>
+        <v>-3.7927491686460826</v>
       </c>
       <c r="O21" s="20">
-        <f t="shared" si="3"/>
-        <v>0.81627775143837411</v>
+        <f t="shared" si="5"/>
+        <v>-1.8381916864608101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>